<commit_message>
Get Company Info. Co-authored-by: 'Fraser McCallum' fraser@themccallums.net.nz
</commit_message>
<xml_diff>
--- a/NZXData.xlsx
+++ b/NZXData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllUniveristy\2022 Uni - Sem2\762\Project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA0E47-FC05-40F7-810A-E938DD46F14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA598CD-100F-46EC-9D8E-767444A77716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7605" yWindow="3030" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="392">
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>NzxCompanyUrl</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Media Contact</t>
+  </si>
+  <si>
+    <t>Auditor</t>
+  </si>
+  <si>
+    <t>Solicitor</t>
+  </si>
+  <si>
+    <t>CFO</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
   <si>
     <t>Ascension Capital Limited</t>
   </si>
@@ -33,6 +57,22 @@
     <t>/companies/ACE</t>
   </si>
   <si>
+    <t xml:space="preserve">
+John Cilliers
+C/o Duncan Cotterill
+Level 2, Tower Building
+50 Customhouse Quay
+Wellington 6143
++64 9 520 1020
+Ascension Capital Limited website</t>
+  </si>
+  <si>
+    <t>BDO Wellington</t>
+  </si>
+  <si>
+    <t>Duncan Cotterill</t>
+  </si>
+  <si>
     <t>AFC Group Holdings Limited</t>
   </si>
   <si>
@@ -1113,10 +1153,83 @@
     <t>/companies/WIN</t>
   </si>
   <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>NzxCompanyUrl</t>
+    <t xml:space="preserve">
+PO Box 230122
+Botany
+Auckland
++6499300245
+AFC Group Holdings Limited website</t>
+  </si>
+  <si>
+    <t>William Buck</t>
+  </si>
+  <si>
+    <t>DLA Piper</t>
+  </si>
+  <si>
+    <t>Hao Long</t>
+  </si>
+  <si>
+    <t>http://www.afcnz.com</t>
+  </si>
+  <si>
+    <t>Mark Freeman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Andrew Porter
+Mail Box 146,
+101 Collins Street,
+Melbourne, VIC 3000
++6139650 9911
+Australian Foundation Investment Company Limited website</t>
+  </si>
+  <si>
+    <t>PriceWaterhouseCoopers</t>
+  </si>
+  <si>
+    <t>Andrew Porter</t>
+  </si>
+  <si>
+    <t>http://www.afi.com.au/</t>
+  </si>
+  <si>
+    <t>Hartley Atkinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Malcolm Tubby
+Level 1
+129 Hurstmere Road
+Takapuna
+Auckland 0622
++64 9 488 0232
+AFT Pharmaceuticals Limited website</t>
+  </si>
+  <si>
+    <t>Deloitte</t>
+  </si>
+  <si>
+    <t>Harmos Horton Lusk Limited</t>
+  </si>
+  <si>
+    <t>http://www.aftpharm.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+John McLean
+PO Box 2959 Wellington 6140
+0800808780
+Smartshares Global Aggregate Bond ETF website</t>
+  </si>
+  <si>
+    <t>KPMG</t>
+  </si>
+  <si>
+    <t>https://smartshares.co.nz/</t>
+  </si>
+  <si>
+    <t>Malcolm Tubby</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1265,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1434,1492 +1550,1583 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B185"/>
+  <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>362</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E3" t="s">
+        <v>374</v>
+      </c>
+      <c r="F3" t="s">
+        <v>375</v>
+      </c>
+      <c r="G3" t="s">
+        <v>376</v>
+      </c>
+      <c r="H3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E4" t="s">
+        <v>380</v>
+      </c>
+      <c r="G4" t="s">
+        <v>381</v>
+      </c>
+      <c r="H4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E5" t="s">
+        <v>385</v>
+      </c>
+      <c r="F5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G5" t="s">
+        <v>391</v>
+      </c>
+      <c r="H5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E6" t="s">
+        <v>389</v>
+      </c>
+      <c r="F6" t="s">
+        <v>375</v>
+      </c>
+      <c r="H6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B76" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B78" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B84" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B86" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B87" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B88" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B89" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B92" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B93" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B94" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="B96" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B97" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B98" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B99" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B100" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B101" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B106" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B107" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="B108" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="B109" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="B110" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="B111" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B112" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="B113" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="B114" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="B115" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="B116" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="B117" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="B118" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B119" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="B120" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="B121" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="B122" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B124" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="B125" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="B126" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B127" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="B128" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="B129" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="B130" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="B131" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="B132" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="B133" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="B134" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="B135" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="B136" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="B137" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="B138" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="B139" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="B140" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="B141" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="B142" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="B143" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="B144" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="B145" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="B146" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="B147" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="B148" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="B149" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="B150" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="B151" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="B152" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="B153" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="B154" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="B155" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="B156" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="B157" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="B158" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="B159" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="B160" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="B161" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="B162" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="B163" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="B164" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="B165" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="B166" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="B167" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="B168" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="B169" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="B170" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="B171" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="B172" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="B173" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="B174" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="B175" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="B176" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B177" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="B178" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="B179" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="B180" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="B181" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="B182" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="B183" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="B184" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="B185" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get Company Info. Co-authored-by: Fraser McCallum <fraser@themccallums.net.nz>
</commit_message>
<xml_diff>
--- a/NZXData.xlsx
+++ b/NZXData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllUniveristy\2022 Uni - Sem2\762\Project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA0E47-FC05-40F7-810A-E938DD46F14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA598CD-100F-46EC-9D8E-767444A77716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7605" yWindow="3030" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="392">
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>NzxCompanyUrl</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Media Contact</t>
+  </si>
+  <si>
+    <t>Auditor</t>
+  </si>
+  <si>
+    <t>Solicitor</t>
+  </si>
+  <si>
+    <t>CFO</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
   <si>
     <t>Ascension Capital Limited</t>
   </si>
@@ -33,6 +57,22 @@
     <t>/companies/ACE</t>
   </si>
   <si>
+    <t xml:space="preserve">
+John Cilliers
+C/o Duncan Cotterill
+Level 2, Tower Building
+50 Customhouse Quay
+Wellington 6143
++64 9 520 1020
+Ascension Capital Limited website</t>
+  </si>
+  <si>
+    <t>BDO Wellington</t>
+  </si>
+  <si>
+    <t>Duncan Cotterill</t>
+  </si>
+  <si>
     <t>AFC Group Holdings Limited</t>
   </si>
   <si>
@@ -1113,10 +1153,83 @@
     <t>/companies/WIN</t>
   </si>
   <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>NzxCompanyUrl</t>
+    <t xml:space="preserve">
+PO Box 230122
+Botany
+Auckland
++6499300245
+AFC Group Holdings Limited website</t>
+  </si>
+  <si>
+    <t>William Buck</t>
+  </si>
+  <si>
+    <t>DLA Piper</t>
+  </si>
+  <si>
+    <t>Hao Long</t>
+  </si>
+  <si>
+    <t>http://www.afcnz.com</t>
+  </si>
+  <si>
+    <t>Mark Freeman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Andrew Porter
+Mail Box 146,
+101 Collins Street,
+Melbourne, VIC 3000
++6139650 9911
+Australian Foundation Investment Company Limited website</t>
+  </si>
+  <si>
+    <t>PriceWaterhouseCoopers</t>
+  </si>
+  <si>
+    <t>Andrew Porter</t>
+  </si>
+  <si>
+    <t>http://www.afi.com.au/</t>
+  </si>
+  <si>
+    <t>Hartley Atkinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Malcolm Tubby
+Level 1
+129 Hurstmere Road
+Takapuna
+Auckland 0622
++64 9 488 0232
+AFT Pharmaceuticals Limited website</t>
+  </si>
+  <si>
+    <t>Deloitte</t>
+  </si>
+  <si>
+    <t>Harmos Horton Lusk Limited</t>
+  </si>
+  <si>
+    <t>http://www.aftpharm.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+John McLean
+PO Box 2959 Wellington 6140
+0800808780
+Smartshares Global Aggregate Bond ETF website</t>
+  </si>
+  <si>
+    <t>KPMG</t>
+  </si>
+  <si>
+    <t>https://smartshares.co.nz/</t>
+  </si>
+  <si>
+    <t>Malcolm Tubby</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1265,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1434,1492 +1550,1583 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B185"/>
+  <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>362</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E3" t="s">
+        <v>374</v>
+      </c>
+      <c r="F3" t="s">
+        <v>375</v>
+      </c>
+      <c r="G3" t="s">
+        <v>376</v>
+      </c>
+      <c r="H3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E4" t="s">
+        <v>380</v>
+      </c>
+      <c r="G4" t="s">
+        <v>381</v>
+      </c>
+      <c r="H4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E5" t="s">
+        <v>385</v>
+      </c>
+      <c r="F5" t="s">
+        <v>386</v>
+      </c>
+      <c r="G5" t="s">
+        <v>391</v>
+      </c>
+      <c r="H5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E6" t="s">
+        <v>389</v>
+      </c>
+      <c r="F6" t="s">
+        <v>375</v>
+      </c>
+      <c r="H6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B71" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="B72" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="B76" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B77" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B78" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B81" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B82" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B84" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B86" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B87" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B88" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B89" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B91" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B92" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B93" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B94" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="B96" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B97" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B98" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B99" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B100" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B101" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B106" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B107" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="B108" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="B109" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="B110" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="B111" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B112" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="B113" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="B114" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="B115" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="B116" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="B117" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="B118" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="B119" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="B120" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="B121" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="B122" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B124" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="B125" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="B126" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B127" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="B128" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="B129" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="B130" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="B131" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="B132" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="B133" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="B134" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="B135" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="B136" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="B137" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="B138" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="B139" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="B140" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="B141" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="B142" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="B143" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="B144" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="B145" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="B146" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="B147" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="B148" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="B149" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="B150" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="B151" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="B152" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="B153" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="B154" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="B155" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="B156" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="B157" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="B158" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="B159" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="B160" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="B161" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="B162" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="B163" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="B164" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="B165" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="B166" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="B167" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="B168" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="B169" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="B170" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="B171" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="B172" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="B173" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="B174" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="B175" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="B176" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B177" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="B178" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="B179" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="B180" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="B181" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="B182" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="B183" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="B184" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="B185" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add browser close after GetCompanyInfo
</commit_message>
<xml_diff>
--- a/NZXData.xlsx
+++ b/NZXData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_UNI_\Infosys 300\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllUniveristy\2022 Uni - Sem2\762\Project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7E3FAD-547B-4198-82B8-6305EC99D9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E67E3EE-787D-485E-97E6-00BF8A30858C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26865" yWindow="6225" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7605" yWindow="3030" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="389">
   <si>
     <t>Ascension Capital Limited</t>
   </si>
@@ -1217,41 +1217,6 @@
   </si>
   <si>
     <t>http://www.aftpharm.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-John McLean
-PO Box 2959 Wellington 6140
-0800808780
-Smartshares Global Aggregate Bond ETF website</t>
-  </si>
-  <si>
-    <t>KPMG</t>
-  </si>
-  <si>
-    <t>https://smartshares.co.nz/</t>
-  </si>
-  <si>
-    <t>Jason Cherrington</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Patrick McCann
-P.O. Box 105675, Auckland 1143, New Zealand
-+64 9 526 8775
-Accordant Group Limited website</t>
-  </si>
-  <si>
-    <t>Deloitte, Auckland</t>
-  </si>
-  <si>
-    <t>MinterEllisonRuddWatts</t>
-  </si>
-  <si>
-    <t>Tony Staub</t>
-  </si>
-  <si>
-    <t>https://accordant.nz/</t>
   </si>
 </sst>
 </file>
@@ -1695,50 +1660,20 @@
         <v>388</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="E6" t="s">
-        <v>390</v>
-      </c>
-      <c r="F6" t="s">
-        <v>375</v>
-      </c>
-      <c r="H6" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>392</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="E7" t="s">
-        <v>394</v>
-      </c>
-      <c r="F7" t="s">
-        <v>395</v>
-      </c>
-      <c r="G7" t="s">
-        <v>396</v>
-      </c>
-      <c r="H7" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add global variable: NumberOfCompaniesToGet
</commit_message>
<xml_diff>
--- a/NZXData.xlsx
+++ b/NZXData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllUniveristy\2022 Uni - Sem2\762\Project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E67E3EE-787D-485E-97E6-00BF8A30858C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A89D853-D6DD-423F-9353-434B9A04997E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7605" yWindow="3030" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="383">
   <si>
     <t>Ascension Capital Limited</t>
   </si>
@@ -1192,31 +1192,6 @@
   </si>
   <si>
     <t>http://www.afi.com.au/</t>
-  </si>
-  <si>
-    <t>Hartley Atkinson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Malcolm Tubby
-Level 1
-129 Hurstmere Road
-Takapuna
-Auckland 0622
-+64 9 488 0232
-AFT Pharmaceuticals Limited website</t>
-  </si>
-  <si>
-    <t>Deloitte</t>
-  </si>
-  <si>
-    <t>Harmos Horton Lusk Limited</t>
-  </si>
-  <si>
-    <t>Malcolm Tubby</t>
-  </si>
-  <si>
-    <t>http://www.aftpharm.com</t>
   </si>
 </sst>
 </file>
@@ -1634,30 +1609,12 @@
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>383</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="E5" t="s">
-        <v>385</v>
-      </c>
-      <c r="F5" t="s">
-        <v>386</v>
-      </c>
-      <c r="G5" t="s">
-        <v>387</v>
-      </c>
-      <c r="H5" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modify file to use MS Edge browser and modify selectors for screenshot. Increased wait timer for screenshot to 3 seconds.
</commit_message>
<xml_diff>
--- a/NZXData.xlsx
+++ b/NZXData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllUniveristy\2022 Uni - Sem2\762\Project\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calvin Kart\Documents\University of Auckland\Engineering\2022\SOFTENG 762\Team Project\Code Repository\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56022ED-FDE3-4E8D-A1BE-95385277D7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E34929-6B8B-42A7-8904-0BF7BCF53C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7605" yWindow="3030" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1494,12 +1494,12 @@
   <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>370</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="174" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>80</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>82</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>102</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>104</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>106</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>108</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>110</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>114</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>116</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>118</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>120</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>122</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>124</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>126</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>128</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>130</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>132</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>134</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>136</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>138</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>140</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>142</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>144</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>146</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>148</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>150</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>152</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>154</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>156</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>158</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>160</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>162</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>164</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>166</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>168</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>170</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>172</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>174</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>174</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>176</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>178</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>180</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>182</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>184</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>184</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>186</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>192</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>194</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>196</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>198</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>200</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>202</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>204</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>206</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>208</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>210</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>212</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>214</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>216</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>218</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>220</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>222</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>224</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>226</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>228</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>230</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>232</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>234</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>236</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>238</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>240</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>242</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>244</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>246</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>248</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>250</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>252</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>254</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>256</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>258</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>260</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>262</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>264</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>266</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>268</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>270</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>272</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>274</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>276</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>278</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>280</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>282</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>284</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>286</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>288</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>290</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>292</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>294</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>296</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>298</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>300</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>302</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>304</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>306</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>308</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>310</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>312</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>314</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>316</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>318</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>320</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>322</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>324</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>326</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>328</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>330</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>332</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>334</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>336</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>338</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>340</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>342</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>344</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>346</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>348</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>350</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>352</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>354</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>358</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>360</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>362</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>364</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>366</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>368</v>
       </c>

</xml_diff>

<commit_message>
Revamped screenshot process, minor change to report production
</commit_message>
<xml_diff>
--- a/NZXData.xlsx
+++ b/NZXData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllUniveristy\2022 Uni - Sem2\762\Project\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_UNI_\Infosys 300\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E9AC1A-E791-48DB-B2C4-FBCC4B1F6E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4887059-C2B5-4FD5-81A7-5DF8459F0A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7605" yWindow="3030" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22770" yWindow="7215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="381">
   <si>
     <t>CompanyName</t>
   </si>
@@ -1153,10 +1153,33 @@
     <t>/companies/WIN</t>
   </si>
   <si>
+    <t xml:space="preserve">
+PO Box 230122
+Botany
+Auckland
++6499300245
+AFC Group Holdings Limited website</t>
+  </si>
+  <si>
+    <t>William Buck</t>
+  </si>
+  <si>
+    <t>DLA Piper</t>
+  </si>
+  <si>
+    <t>Hao Long</t>
+  </si>
+  <si>
+    <t>http://www.afcnz.com</t>
+  </si>
+  <si>
     <t>Screenshots</t>
   </si>
   <si>
     <t>unavailable</t>
+  </si>
+  <si>
+    <t>companyScreenshots\I3.png</t>
   </si>
 </sst>
 </file>
@@ -1479,11 +1502,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1511,7 +1538,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="315" x14ac:dyDescent="0.25">
@@ -1531,15 +1558,33 @@
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E3" t="s">
+        <v>374</v>
+      </c>
+      <c r="F3" t="s">
+        <v>375</v>
+      </c>
+      <c r="G3" t="s">
+        <v>376</v>
+      </c>
+      <c r="H3" t="s">
+        <v>377</v>
+      </c>
+      <c r="I3" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add documentation to main workflow
</commit_message>
<xml_diff>
--- a/NZXData.xlsx
+++ b/NZXData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllUniveristy\2022 Uni - Sem2\762\Project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60D8164-BC68-45DF-889D-41508098D8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEF324A-5CBE-483B-846B-7F091DDC4B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7605" yWindow="3030" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="381">
   <si>
     <t>CompanyName</t>
   </si>
@@ -1173,27 +1173,6 @@
     <t>http://www.afcnz.com</t>
   </si>
   <si>
-    <t>Mark Freeman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Andrew Porter
-Mail Box 146,
-101 Collins Street,
-Melbourne, VIC 3000
-+6139650 9911
-Australian Foundation Investment Company Limited website</t>
-  </si>
-  <si>
-    <t>PriceWaterhouseCoopers</t>
-  </si>
-  <si>
-    <t>Andrew Porter</t>
-  </si>
-  <si>
-    <t>http://www.afi.com.au/</t>
-  </si>
-  <si>
     <t>Screenshots</t>
   </si>
   <si>
@@ -1201,9 +1180,6 @@
   </si>
   <si>
     <t>companyScreenshots\I3.png</t>
-  </si>
-  <si>
-    <t>companyScreenshots\I4.png</t>
   </si>
 </sst>
 </file>
@@ -1558,7 +1534,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="315" x14ac:dyDescent="0.25">
@@ -1578,7 +1554,7 @@
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -1604,33 +1580,15 @@
         <v>377</v>
       </c>
       <c r="I3" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="330" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>378</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="E4" t="s">
-        <v>380</v>
-      </c>
-      <c r="G4" t="s">
-        <v>381</v>
-      </c>
-      <c r="H4" t="s">
-        <v>382</v>
-      </c>
-      <c r="I4" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>